<commit_message>
add NIH ebola challenge synthetic data
</commit_message>
<xml_diff>
--- a/data/__table_epievent_template.xlsx
+++ b/data/__table_epievent_template.xlsx
@@ -5,7 +5,7 @@
   <fileSharing readOnlyRecommended="1"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="38880" yWindow="3500" windowWidth="25600" windowHeight="17560" tabRatio="500"/>
+    <workbookView xWindow="6340" yWindow="5380" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="cholera_Haiti_2010.csv" sheetId="1" r:id="rId1"/>
@@ -74,7 +74,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -94,6 +94,14 @@
       <u/>
       <sz val="12"/>
       <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -125,10 +133,18 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -469,73 +485,88 @@
   <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:M55"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" showRuler="0" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.83203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:13">
-      <c r="A1" t="s">
+    <row r="1" spans="1:13" s="2" customFormat="1">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
-      <c r="A2">
+    <row r="2" spans="1:13" s="3" customFormat="1">
+      <c r="A2" s="3">
         <v>999</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="3">
         <v>9999</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="3">
         <v>0</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="L2">
+      <c r="L2" s="3">
         <v>0</v>
       </c>
-      <c r="M2" t="s">
+      <c r="M2" s="3" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>